<commit_message>
Modify each report such that they can be run for an individual Relationship or an entire Bid Pool.
</commit_message>
<xml_diff>
--- a/Src/SummitReports.Objects/Reports/LoansReportPres/LoansReportPres.xlsx
+++ b/Src/SummitReports.Objects/Reports/LoansReportPres/LoansReportPres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajoyce\Documents\GitHub\SummitReports\Src\SummitReports.Objects\Reports\LoansReportPres\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E9BDF3-A483-43CC-A582-1CE110FADF19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE97139-BE56-40D9-88B7-1CC061FF729C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3465" yWindow="3465" windowWidth="21585" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Loan Data</t>
-  </si>
-  <si>
-    <t>Bid Sub Pool</t>
-  </si>
-  <si>
-    <t>Relationship Name</t>
   </si>
   <si>
     <t>Short Name</t>
@@ -565,46 +559,49 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M7"/>
+  <dimension ref="B1:K9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
     <col min="3" max="3" width="36.5703125" customWidth="1"/>
     <col min="4" max="4" width="41.140625" customWidth="1"/>
     <col min="5" max="5" width="43.42578125" customWidth="1"/>
-    <col min="6" max="6" width="46.28515625" customWidth="1"/>
-    <col min="7" max="7" width="45.7109375" customWidth="1"/>
+    <col min="6" max="7" width="19.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="12" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
     <col min="13" max="13" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="25.5" customHeight="1">
+    <row r="1" spans="2:11" ht="25.5" customHeight="1">
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="2:13" ht="3.95" customHeight="1"/>
-    <row r="3" spans="2:13" ht="18" customHeight="1">
+    <row r="2" spans="2:11" ht="3.95" customHeight="1"/>
+    <row r="3" spans="2:11" ht="18" customHeight="1">
       <c r="B3" s="4"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="2:13" ht="5.0999999999999996" customHeight="1"/>
-    <row r="5" spans="2:13" ht="11.85" customHeight="1"/>
-    <row r="6" spans="2:13">
+    <row r="4" spans="2:11" ht="5.0999999999999996" customHeight="1"/>
+    <row r="5" spans="2:11" ht="11.85" customHeight="1"/>
+    <row r="6" spans="2:11" ht="15" customHeight="1">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -628,20 +625,16 @@
       <c r="K6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="7" spans="2:13" ht="27.4" customHeight="1"/>
+    <row r="7" spans="2:11" ht="15" customHeight="1"/>
+    <row r="8" spans="2:11" ht="15" customHeight="1"/>
+    <row r="9" spans="2:11" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="41" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>